<commit_message>
rename test cases name
</commit_message>
<xml_diff>
--- a/src/test/resources/addstudent.xlsx
+++ b/src/test/resources/addstudent.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>Hung</t>
   </si>
@@ -26,9 +26,6 @@
   </si>
   <si>
     <t>December</t>
-  </si>
-  <si>
-    <t>hungnxv1</t>
   </si>
   <si>
     <t>Vinh 1</t>
@@ -343,16 +340,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>12345.0</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="E2" s="1">
+        <v>123456.0</v>
       </c>
       <c r="F2" s="1">
         <v>7.0</v>
@@ -372,14 +366,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1">
         <v>7.0</v>
@@ -391,7 +381,7 @@
         <v>2010.0</v>
       </c>
       <c r="I3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -399,13 +389,10 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1">
-        <v>123456.0</v>
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="F4" s="1">
         <v>7.0</v>
@@ -417,7 +404,7 @@
         <v>2010.0</v>
       </c>
       <c r="I4" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -425,16 +412,16 @@
         <v>0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1">
-        <v>7.0</v>
+        <v>31.0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="H5" s="1">
         <v>2010.0</v>
@@ -451,7 +438,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F6" s="1">
         <v>7.0</v>
@@ -460,55 +447,9 @@
         <v>4</v>
       </c>
       <c r="H6" s="1">
-        <v>2010.0</v>
+        <v>2030.0</v>
       </c>
       <c r="I6" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="1">
-        <v>2010.0</v>
-      </c>
-      <c r="I7" s="1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="1">
-        <v>2030.0</v>
-      </c>
-      <c r="I8" s="1" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>